<commit_message>
Update python tool 'prog_parser.py' and example.
</commit_message>
<xml_diff>
--- a/usr/tool/python/prog_parser_sample/reg_table.xlsx
+++ b/usr/tool/python/prog_parser_sample/reg_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -313,19 +313,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="12"/>
@@ -685,15 +682,17 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <pane xSplit="5" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="40.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="38.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="40.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="4" width="12.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="2" width="11.52"/>
   </cols>
@@ -771,7 +770,6 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="5" t="s">
@@ -983,6 +981,9 @@
       <c r="D14" s="19" t="s">
         <v>31</v>
       </c>
+      <c r="E14" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="F14" s="20" t="n">
         <v>0</v>
       </c>
@@ -1006,6 +1007,9 @@
       <c r="D15" s="19" t="s">
         <v>31</v>
       </c>
+      <c r="E15" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="F15" s="20" t="n">
         <v>0</v>
       </c>
@@ -1028,6 +1032,9 @@
       </c>
       <c r="D16" s="19" t="s">
         <v>31</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="F16" s="20" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Update progparser & sample code.
</commit_message>
<xml_diff>
--- a/usr/tool/python/prog_parser_sample/reg_table.xlsx
+++ b/usr/tool/python/prog_parser_sample/reg_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="117">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t xml:space="preserve">FileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_reg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_reg3</t>
   </si>
   <si>
     <t xml:space="preserve">Eng.</t>
@@ -121,6 +130,15 @@
   <si>
     <t xml:space="preserve">AGE_CYCLE_COUNTER
 cycle count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">378</t>
   </si>
   <si>
     <t xml:space="preserve">0xc</t>
@@ -170,6 +188,9 @@
 3: 96x64</t>
   </si>
   <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
     <t xml:space="preserve">13_12</t>
   </si>
   <si>
@@ -261,6 +282,12 @@
     <t xml:space="preserve">SRC1_C0_WIDTH</t>
   </si>
   <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
     <t xml:space="preserve">22_20</t>
   </si>
   <si>
@@ -351,10 +378,22 @@
     <t xml:space="preserve">SRC1_CONST_ALPHA</t>
   </si>
   <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
     <t xml:space="preserve">31_24</t>
   </si>
   <si>
     <t xml:space="preserve">SRC1_CONST_ALPHA_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
   </si>
   <si>
     <t xml:space="preserve">0x40</t>
@@ -519,15 +558,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -545,6 +580,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,6 +603,10 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,6 +624,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -600,10 +647,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -614,6 +657,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -729,632 +776,1045 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="24.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="9.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="37.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="7.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="10.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="7.91"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="5" t="s">
+    <row r="1" s="6" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" s="6" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="E3" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="E4" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4"/>
-      <c r="E5" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="3"/>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="17"/>
-      <c r="C8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="18" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" s="17" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="17"/>
-      <c r="C9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="18" t="s">
+      <c r="C7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="F7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" s="18" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="17"/>
-      <c r="C10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="18" t="s">
+      <c r="E8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="F8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" s="18" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="19"/>
+      <c r="C9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" s="16" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="18" t="s">
+      <c r="E9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="F9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" s="18" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="E10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="F10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" s="18" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="19"/>
+      <c r="C11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="E11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="F11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" s="24" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="s">
+      <c r="B12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="C12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="E12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="23" t="s">
+      <c r="F12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" s="26" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="B13" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="C13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
+      <c r="D13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="F13" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="22" t="s">
+      <c r="G13" s="25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="26"/>
-      <c r="C16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="18" t="s">
+      <c r="H13" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="27" t="s">
+    </row>
+    <row r="14" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="26"/>
-      <c r="C17" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="18" t="s">
+      <c r="B14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="C14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" s="26" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" s="25" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="26"/>
-      <c r="C18" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="18" t="s">
+      <c r="B15" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="C15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" s="25" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="26"/>
-      <c r="C19" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="28" t="s">
+      <c r="F15" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="28"/>
+      <c r="C16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="29" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="26"/>
-      <c r="C20" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="29" t="s">
+      <c r="F16" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="28"/>
+      <c r="C17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E17" s="29" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="26"/>
-      <c r="C21" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="29" t="s">
+      <c r="F17" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" s="27" customFormat="true" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="28"/>
+      <c r="C18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E18" s="30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="26"/>
-      <c r="C22" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="29" t="s">
+      <c r="F18" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" s="27" customFormat="true" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="28"/>
+      <c r="C19" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E19" s="30" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="26"/>
-      <c r="C23" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="29" t="s">
+      <c r="F19" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="27" t="s">
+    </row>
+    <row r="20" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="28"/>
+      <c r="C20" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="31" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" s="25" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="26"/>
-      <c r="C24" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="29" t="s">
+      <c r="E20" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="F20" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="28"/>
+      <c r="C21" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="31" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" s="25" customFormat="true" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="26"/>
-      <c r="C25" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="29" t="s">
+      <c r="E21" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="F21" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="28"/>
+      <c r="C22" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="31" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" s="24" customFormat="true" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="s">
+      <c r="E22" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="F22" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="28"/>
+      <c r="C23" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="30" t="s">
+      <c r="E23" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="F23" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" s="27" customFormat="true" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="28"/>
+      <c r="C24" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="26"/>
-      <c r="C27" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="27" t="s">
+      <c r="E24" s="30" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" s="25" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="26"/>
-      <c r="C28" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="29" t="s">
+      <c r="F24" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" s="27" customFormat="true" ht="57.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="28"/>
+      <c r="C25" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E25" s="30" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="29" s="25" customFormat="true" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="26"/>
-      <c r="C29" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="29" t="s">
+      <c r="F25" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" s="26" customFormat="true" ht="43.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="B26" s="23" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="30" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="26"/>
-      <c r="C30" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" s="27" t="s">
+      <c r="C26" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="32" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="26"/>
-      <c r="C31" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="29" t="s">
+      <c r="E26" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="F26" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="28"/>
+      <c r="C27" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="26"/>
-      <c r="C32" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="29" t="s">
+      <c r="F27" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" s="27" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="28"/>
+      <c r="C28" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E28" s="30" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="33" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="26"/>
-      <c r="C33" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="29" t="s">
+      <c r="F28" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" s="27" customFormat="true" ht="57.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="28"/>
+      <c r="C29" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E29" s="30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="26"/>
-      <c r="C34" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="29" t="s">
+      <c r="F29" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="28"/>
+      <c r="C30" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="F30" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="28"/>
+      <c r="C31" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="26"/>
-      <c r="C35" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="29" t="s">
+      <c r="E31" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="F31" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="28"/>
+      <c r="C32" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="31" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="36" s="24" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="21" t="s">
+      <c r="E32" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="F32" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="23" t="s">
+      <c r="H32" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="26"/>
-      <c r="C37" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="29" t="s">
+    <row r="33" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="28"/>
+      <c r="C33" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E33" s="29" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="26"/>
-      <c r="C38" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="27" t="s">
+      <c r="F33" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="28"/>
+      <c r="C34" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="31" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="39" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="26"/>
-      <c r="C39" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="29" t="s">
+      <c r="E34" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="F34" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="28"/>
+      <c r="C35" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="31" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" s="25" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="26"/>
-      <c r="C40" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="28" t="s">
+      <c r="E35" s="29" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="41" s="25" customFormat="true" ht="71.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="26"/>
-      <c r="C41" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E41" s="28" t="s">
+      <c r="F35" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" s="26" customFormat="true" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="26"/>
-      <c r="C42" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="29" t="s">
+      <c r="B36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="27" t="s">
+      <c r="C36" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="24" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="26"/>
-      <c r="C43" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="29" t="s">
+      <c r="F36" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="28"/>
+      <c r="C37" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="27" t="s">
+      <c r="E37" s="29" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="44" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="26"/>
-      <c r="C44" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="29" t="s">
+      <c r="F37" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="28"/>
+      <c r="C38" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="27" t="s">
+      <c r="F38" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="28"/>
+      <c r="C39" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="31" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="26"/>
-      <c r="C45" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="29" t="s">
+      <c r="E39" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="27" t="s">
+      <c r="F39" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" s="27" customFormat="true" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="28"/>
+      <c r="C40" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="46" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="26"/>
-      <c r="C46" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="18" t="s">
+      <c r="F40" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" s="27" customFormat="true" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="28"/>
+      <c r="C41" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="27" t="s">
+      <c r="F41" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="28"/>
+      <c r="C42" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="31" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="47" s="25" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="26"/>
-      <c r="C47" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="18" t="s">
+      <c r="E42" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="E47" s="27" t="s">
+      <c r="F42" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="28"/>
+      <c r="C43" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="31" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="48" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="11" t="s">
+      <c r="E43" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="F43" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="28"/>
+      <c r="C44" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="20" t="s">
+      <c r="E44" s="29" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="49" s="31" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="31" t="s">
+      <c r="F44" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G44" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" s="28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="28"/>
+      <c r="C45" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="E49" s="32"/>
+      <c r="E45" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H45" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="28"/>
+      <c r="C46" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="G46" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" s="27" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="28"/>
+      <c r="C47" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="G47" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H47" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" s="17" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" s="33" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>